<commit_message>
Wijziging van kolomnamen uppercase en lowercase en testen
</commit_message>
<xml_diff>
--- a/src/basiskaart/fixtures/wms_kaart_database.xlsx
+++ b/src/basiskaart/fixtures/wms_kaart_database.xlsx
@@ -15,6 +15,8 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -70,7 +72,7 @@
     <t xml:space="preserve">punt</t>
   </si>
   <si>
-    <t xml:space="preserve">lokaalid, bgttype, plustype</t>
+    <t xml:space="preserve">identificatie_lokaalid, bgt_type, plus_type</t>
   </si>
   <si>
     <t xml:space="preserve">BGTPLUS_BAK_afval_apart_plaats</t>
@@ -115,7 +117,7 @@
     <t xml:space="preserve">BGTPLUS_KDL_keermuur</t>
   </si>
   <si>
-    <t xml:space="preserve">BGTPLUS_KST_cai-kast</t>
+    <t xml:space="preserve">BGTPLUS_KST_cai_kast</t>
   </si>
   <si>
     <t xml:space="preserve">BGTPLUS_KST_elektrakast</t>
@@ -163,10 +165,10 @@
     <t xml:space="preserve">BGTPLUS_PAL_lichtmast</t>
   </si>
   <si>
-    <t xml:space="preserve">BGTPLUS_PUT_brandkraan_-put</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BGTPLUS_PUT_inspectie-_rioolput</t>
+    <t xml:space="preserve">BGTPLUS_PUT_brandkraan__put</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGTPLUS_PUT_inspectie__rioolput</t>
   </si>
   <si>
     <t xml:space="preserve">BGTPLUS_PUT_kolk</t>
@@ -244,7 +246,7 @@
     <t xml:space="preserve">terreindeel</t>
   </si>
   <si>
-    <t xml:space="preserve">lokaalid, bgtfysvkn, plusfyskvkn</t>
+    <t xml:space="preserve">identificatie_lokaalid, bgt_fysiekvoorkomen, plus_fysiekvoorkomen</t>
   </si>
   <si>
     <t xml:space="preserve">BGT_BTRN_bouwland</t>
@@ -376,7 +378,7 @@
     <t xml:space="preserve">wegdeel</t>
   </si>
   <si>
-    <t xml:space="preserve">lokaalid, bgtfunctie, plusfunct</t>
+    <t xml:space="preserve">identificatie_lokaalid, bgt_functie, plus_functie</t>
   </si>
   <si>
     <t xml:space="preserve">BGT_OWGL_transitie</t>
@@ -448,7 +450,7 @@
     <t xml:space="preserve">BGT_WGL_inrit</t>
   </si>
   <si>
-    <t xml:space="preserve">BGT_WGL_ov-baan</t>
+    <t xml:space="preserve">BGT_WGL_ov_baan</t>
   </si>
   <si>
     <t xml:space="preserve">BGT_WGL_overweg</t>
@@ -758,24 +760,24 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B114" activeCellId="0" sqref="B114"/>
+      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10:I11 I111 I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="44.2186234817814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="23.6518218623482"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.5101214574899"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="45.4736842105263"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="62.3846153846154"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="44.9028340080972"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="25.5951417004049"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="20.1093117408907"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="10.2834008097166"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -810,7 +812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -5268,7 +5270,7 @@
   <autoFilter ref="A1:J132"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5285,17 +5287,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="3" sqref="I10:I11 I111 I127 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5311,17 +5313,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="3" sqref="I10:I11 I111 I127 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Typo's gecorrigeerd in wms_kaart_database.xlsx
</commit_message>
<xml_diff>
--- a/src/basiskaart/fixtures/wms_kaart_database.xlsx
+++ b/src/basiskaart/fixtures/wms_kaart_database.xlsx
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -117,7 +118,7 @@
     <t xml:space="preserve">BGTPLUS_KDL_keermuur</t>
   </si>
   <si>
-    <t xml:space="preserve">BGTPLUS_KST_cai_kast</t>
+    <t xml:space="preserve">BGTPLUS_KST_cai-kast</t>
   </si>
   <si>
     <t xml:space="preserve">BGTPLUS_KST_elektrakast</t>
@@ -165,10 +166,10 @@
     <t xml:space="preserve">BGTPLUS_PAL_lichtmast</t>
   </si>
   <si>
-    <t xml:space="preserve">BGTPLUS_PUT_brandkraan__put</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BGTPLUS_PUT_inspectie__rioolput</t>
+    <t xml:space="preserve">BGTPLUS_PUT_brandkraan_-put</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGTPLUS_PUT_inspectie-_rioolput</t>
   </si>
   <si>
     <t xml:space="preserve">BGTPLUS_PUT_kolk</t>
@@ -450,7 +451,7 @@
     <t xml:space="preserve">BGT_WGL_inrit</t>
   </si>
   <si>
-    <t xml:space="preserve">BGT_WGL_ov_baan</t>
+    <t xml:space="preserve">BGT_WGL_ov-baan</t>
   </si>
   <si>
     <t xml:space="preserve">BGT_WGL_overweg</t>
@@ -760,24 +761,24 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10:I11 I111 I127"/>
+      <selection pane="bottomLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="44.2186234817814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="23.6518218623482"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.5101214574899"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="45.4736842105263"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="62.3846153846154"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="44.9028340080972"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="25.5951417004049"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="20.1093117408907"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="61.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5270,7 +5271,7 @@
   <autoFilter ref="A1:J132"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5287,17 +5288,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="3" sqref="I10:I11 I111 I127 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.58673469387755"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5313,17 +5314,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="3" sqref="I10:I11 I111 I127 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.58673469387755"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Ontbrekende geometrie in de views
</commit_message>
<xml_diff>
--- a/src/basiskaart/fixtures/wms_kaart_database.xlsx
+++ b/src/basiskaart/fixtures/wms_kaart_database.xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Blad1!$A$1:$J$132</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -73,7 +74,7 @@
     <t xml:space="preserve">punt</t>
   </si>
   <si>
-    <t xml:space="preserve">identificatie_lokaalid, bgt_type, plus_type</t>
+    <t xml:space="preserve">identificatie_lokaalid, bgt_type, plus_type, geometrie</t>
   </si>
   <si>
     <t xml:space="preserve">BGTPLUS_BAK_afval_apart_plaats</t>
@@ -247,7 +248,7 @@
     <t xml:space="preserve">terreindeel</t>
   </si>
   <si>
-    <t xml:space="preserve">identificatie_lokaalid, bgt_fysiekvoorkomen, plus_fysiekvoorkomen</t>
+    <t xml:space="preserve">identificatie_lokaalid, bgt_fysiekvoorkomen, plus_fysiekvoorkomen, geometrie</t>
   </si>
   <si>
     <t xml:space="preserve">BGT_BTRN_bouwland</t>
@@ -379,7 +380,7 @@
     <t xml:space="preserve">wegdeel</t>
   </si>
   <si>
-    <t xml:space="preserve">identificatie_lokaalid, bgt_functie, plus_functie</t>
+    <t xml:space="preserve">identificatie_lokaalid, bgt_functie, plus_functie, geometrie</t>
   </si>
   <si>
     <t xml:space="preserve">BGT_OWGL_transitie</t>
@@ -760,25 +761,25 @@
   </sheetPr>
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F132" activeCellId="0" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="61.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="43.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="61.015306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="7" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3567,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
@@ -5199,7 +5200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>10</v>
       </c>
@@ -5293,7 +5294,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.44897959183673"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5319,7 +5320,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.44897959183673"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>